<commit_message>
Checked grapfics for bubblesort
</commit_message>
<xml_diff>
--- a/comparison_of_sorting_algorithms.xlsx
+++ b/comparison_of_sorting_algorithms.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github-CSharp\Sorting Algorithms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github-C\SortingAlgosTimeComp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E61752A-5E32-4B2C-B7DF-96188FF78771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987950F2-489B-46CF-9598-12B1E6EAA7DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -250,12 +250,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -263,6 +257,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,24 +358,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -392,16 +374,16 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>7544</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -471,24 +453,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -498,24 +462,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -584,24 +530,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -611,24 +539,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -697,24 +607,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -783,24 +675,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1845,15 +1719,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2147,7 +2021,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2161,17 +2035,17 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="7"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4">
@@ -2189,12 +2063,12 @@
       <c r="F2" s="4">
         <v>500000</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="7">
         <v>1000000</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3">
@@ -2204,112 +2078,64 @@
         <v>2</v>
       </c>
       <c r="D3" s="3">
-        <v>3</v>
+        <v>7544</v>
       </c>
       <c r="E3" s="3">
         <v>4</v>
       </c>
       <c r="F3" s="3">
+        <v>4</v>
+      </c>
+      <c r="G3" s="9">
         <v>5</v>
       </c>
-      <c r="G3" s="11">
+    </row>
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="3">
-        <v>3</v>
-      </c>
-      <c r="F4" s="3">
-        <v>4</v>
-      </c>
-      <c r="G4" s="11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3">
-        <v>2</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3">
-        <v>3</v>
-      </c>
-      <c r="E5" s="3">
-        <v>4</v>
-      </c>
-      <c r="F5" s="3">
-        <v>6</v>
-      </c>
-      <c r="G5" s="11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="3">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3">
-        <v>4</v>
-      </c>
-      <c r="F6" s="3">
-        <v>5</v>
-      </c>
-      <c r="G6" s="11">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3">
-        <v>3</v>
-      </c>
-      <c r="D7" s="3">
-        <v>2</v>
-      </c>
-      <c r="E7" s="3">
-        <v>5</v>
-      </c>
-      <c r="F7" s="3">
-        <v>4</v>
-      </c>
-      <c r="G7" s="11">
-        <v>6</v>
-      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="3"/>
@@ -2317,32 +2143,32 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="11"/>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="14"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="7"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="4">
@@ -2360,23 +2186,25 @@
       <c r="F11" s="4">
         <v>500000</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="7">
         <v>1000000</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3">
+        <v>3436</v>
+      </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="11"/>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="3"/>
@@ -2384,10 +2212,10 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="11"/>
+      <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="3"/>
@@ -2395,10 +2223,10 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="11"/>
+      <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="3"/>
@@ -2406,10 +2234,10 @@
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="11"/>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="3"/>
@@ -2417,10 +2245,10 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="11"/>
+      <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="3"/>
@@ -2428,32 +2256,32 @@
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="11"/>
+      <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="14"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="12"/>
     </row>
     <row r="19" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="7"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B20" s="4">
@@ -2471,23 +2299,25 @@
       <c r="F20" s="4">
         <v>500000</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="7">
         <v>1000000</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3">
+        <v>6108</v>
+      </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="11"/>
+      <c r="G21" s="9"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B22" s="3"/>
@@ -2495,10 +2325,10 @@
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="11"/>
+      <c r="G22" s="9"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="3"/>
@@ -2506,11 +2336,11 @@
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="11"/>
+      <c r="G23" s="9"/>
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="3"/>
@@ -2518,10 +2348,10 @@
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="11"/>
+      <c r="G24" s="9"/>
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B25" s="3"/>
@@ -2529,10 +2359,10 @@
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="11"/>
+      <c r="G25" s="9"/>
     </row>
     <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B26" s="3"/>
@@ -2540,18 +2370,18 @@
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="11"/>
+      <c r="G26" s="9"/>
     </row>
     <row r="27" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="14"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="12"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A9">

</xml_diff>